<commit_message>
OPTN 20 year kidney survival data
</commit_message>
<xml_diff>
--- a/output/LEGEND_Figures_C1_C2_Deceased.xlsx
+++ b/output/LEGEND_Figures_C1_C2_Deceased.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathleen/Courses/Berkeley-Data-Analytics/Class-Work/repos/transplant-survival/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B37533A-F17B-8145-8FDF-E7A57F148E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A889433-FCA5-EF4F-BCE9-F77B69FE6B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="800" windowWidth="21220" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="800" windowWidth="34660" windowHeight="19520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Columns" sheetId="1" r:id="rId1"/>
+    <sheet name="Database columns" sheetId="2" r:id="rId2"/>
+    <sheet name="Graft Survival Columns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="486">
   <si>
     <t xml:space="preserve"> CTR_CD</t>
   </si>
@@ -1151,15 +1153,349 @@
   </si>
   <si>
     <t xml:space="preserve"> Primary  Disease (Percent)Valvular Heart Disease | region</t>
+  </si>
+  <si>
+    <t>'ENTIRE_NAME', </t>
+  </si>
+  <si>
+    <t>'CTR_CD', </t>
+  </si>
+  <si>
+    <t>‘CTR_TY', </t>
+  </si>
+  <si>
+    <t>'RELEASE_DATE', </t>
+  </si>
+  <si>
+    <t>'ORG', </t>
+  </si>
+  <si>
+    <t>'RCC_A10_C',</t>
+  </si>
+  <si>
+    <t>'RCC_A17_C', </t>
+  </si>
+  <si>
+    <t>'RCC_A2_C', </t>
+  </si>
+  <si>
+    <t>'RCC_A34_C', </t>
+  </si>
+  <si>
+    <t>'RC_A49_C', </t>
+  </si>
+  <si>
+    <t>'RCC_A65P_C', </t>
+  </si>
+  <si>
+    <t>'RCC_AU_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BAB_C',</t>
+  </si>
+  <si>
+    <t>'RCC_BA_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BB_C',</t>
+  </si>
+  <si>
+    <t>'RCC_BO_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BMI20_C',</t>
+  </si>
+  <si>
+    <t>'RCC_BMI25_C',</t>
+  </si>
+  <si>
+    <t>'RCC_BMI30_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BMI31P_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BMINR_C', </t>
+  </si>
+  <si>
+    <t>'RCC_BU_C', </t>
+  </si>
+  <si>
+    <t>'RCC_GF_C',</t>
+  </si>
+  <si>
+    <t>'RCC_GM_C', </t>
+  </si>
+  <si>
+    <t>'RCC_GU_C', </t>
+  </si>
+  <si>
+    <t>'RCC_ICU_C', </t>
+  </si>
+  <si>
+    <t>'RCC_HOSPNR_C', </t>
+  </si>
+  <si>
+    <t>'RCC_HOSP_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PTXN_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PTXU_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PTXY_C',</t>
+  </si>
+  <si>
+    <t>'RCC_NOTHOSP_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1A_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1A_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1B_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST1B_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST2_C',</t>
+  </si>
+  <si>
+    <t>'RCC_TST2_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST2A_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST2A_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST2B_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST2B_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TST3_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TST3_R', </t>
+  </si>
+  <si>
+    <t>'RCC_ME11_C',</t>
+  </si>
+  <si>
+    <t>'RCC_ME11_R', </t>
+  </si>
+  <si>
+    <t>'RCC_ME15_C',</t>
+  </si>
+  <si>
+    <t>'RCC_ME15_R', </t>
+  </si>
+  <si>
+    <t>'RCC_ME21_C', </t>
+  </si>
+  <si>
+    <t>'RCC_ME21_R', </t>
+  </si>
+  <si>
+    <t>'RCC_ME31_C', </t>
+  </si>
+  <si>
+    <t>'RCC_ME31_R', </t>
+  </si>
+  <si>
+    <t>'RCC_ME6_C',</t>
+  </si>
+  <si>
+    <t>'RCC_ME6_R', </t>
+  </si>
+  <si>
+    <t>'RCC_PE6_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PE6_R', </t>
+  </si>
+  <si>
+    <t>'RCC_PE11_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PE11_R', </t>
+  </si>
+  <si>
+    <t>'RCC_PE15_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PE15_R', </t>
+  </si>
+  <si>
+    <t>'RCC_PE21_C',</t>
+  </si>
+  <si>
+    <t>'RCC_PE21_R', </t>
+  </si>
+  <si>
+    <t>'RCC_PE31_C', </t>
+  </si>
+  <si>
+    <t>'RCC_PE31_R', </t>
+  </si>
+  <si>
+    <t>'RCC_TINA_C', </t>
+  </si>
+  <si>
+    <t>'RCC_TINA_R', </t>
+  </si>
+  <si>
+    <t>'RCC_N_C’, </t>
+  </si>
+  <si>
+    <t>'YEAR',</t>
+  </si>
+  <si>
+    <t>'MONTH', </t>
+  </si>
+  <si>
+    <t>'D_OR_L'</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Deceased or Living</t>
+  </si>
+  <si>
+    <t>RCC_DEVS_C</t>
+  </si>
+  <si>
+    <t>Recipient Mechanical, Ventilated or Organ-Perfusion Support Status at Transplant (Percent)Devices * | center</t>
+  </si>
+  <si>
+    <t>RCC_NOTLS_C</t>
+  </si>
+  <si>
+    <t>Recipient Mechanical, Ventilated or Organ-Perfusion Support Status at Transplant (Percent)No Support Mechanism | center</t>
+  </si>
+  <si>
+    <t>RCC_LS_C</t>
+  </si>
+  <si>
+    <t>Recipient Mechanical, Ventilated or Organ-Perfusion Support Status at Transplant (Percent)Other Support Mechanism | center</t>
+  </si>
+  <si>
+    <t>RCC_LSNR_C</t>
+  </si>
+  <si>
+    <t>Recipient Mechanical, Ventilated or Organ-Perfusion Support Status at Transplant (Percent)Unknown | center</t>
+  </si>
+  <si>
+    <t>‘RCC_A64_C, </t>
+  </si>
+  <si>
+    <t>Tables C9, C14; Figures C9-C10, C19-C20</t>
+  </si>
+  <si>
+    <t>Graft survival (3-Year Cohort)</t>
+  </si>
+  <si>
+    <t>Undergone transplant</t>
+  </si>
+  <si>
+    <t>Ends follow-up on 3/12/2020 for recipients transplanted prior to 3/13/2020</t>
+  </si>
+  <si>
+    <t>Tables C15-C16, C18-C19; Figures C21-C22, C23-C24</t>
+  </si>
+  <si>
+    <t>Patient survival (1-Year Cohort)</t>
+  </si>
+  <si>
+    <t>Undergone transplant </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Tables C17, C20; Figures C25-C26, C31-C32</t>
+  </si>
+  <si>
+    <t>Patient survival (3-Year Cohort)</t>
+  </si>
+  <si>
+    <t>Figure or Table No.</t>
+  </si>
+  <si>
+    <t>Figure or Table Title</t>
+  </si>
+  <si>
+    <t>Reference population</t>
+  </si>
+  <si>
+    <t>Cohort Begin Date</t>
+  </si>
+  <si>
+    <t>Cohort End Date</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>Cohorts Evaluated in the Fall 2023 PSR Cycle</t>
+  </si>
+  <si>
+    <t>Tables C5, C10; Figures C1-C2, C11-C12</t>
+  </si>
+  <si>
+    <t>Graft survival (1-Month Cohort)</t>
+  </si>
+  <si>
+    <t>Tables C6, C11; Figures C3-C4, C13-C14</t>
+  </si>
+  <si>
+    <t>Graft survival (90-Day Cohort)</t>
+  </si>
+  <si>
+    <t>Tables C7, C12; Figures C5-C6, C15-C16</t>
+  </si>
+  <si>
+    <t>Graft survival (1-Year Cohort)</t>
+  </si>
+  <si>
+    <t>Tables C8, C13; Figures C7-C8, C17-C18</t>
+  </si>
+  <si>
+    <t>Graft survival (1-Year Conditional on 90-Days Cohort)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1179,6 +1515,70 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF323232"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF323232"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF070072"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1216,12 +1616,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,201 +1967,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B191"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C72" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="63" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="20">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="20">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="20">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="20">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="20">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="20">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="20">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="20">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="20">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="20">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="20">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="20">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="20">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="20">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="20">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="20">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="20">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="20">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="20">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="20">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="20">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="20">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1728,7 +2206,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1736,151 +2214,178 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="20">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" ht="20">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="20">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" ht="20">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="20">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" ht="20">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="20">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" ht="20">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="20">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" ht="20">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="20">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" ht="20">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" ht="20">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" ht="20">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" ht="20">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="3"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" ht="20">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" ht="20">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" ht="20">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1888,7 +2393,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1896,7 +2401,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1904,7 +2409,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1912,7 +2417,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1920,7 +2425,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1928,7 +2433,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1936,7 +2441,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1944,7 +2449,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -1952,7 +2457,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +2465,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1968,7 +2473,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -1976,7 +2481,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -1984,7 +2489,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -1992,7 +2497,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -2000,7 +2505,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -2008,7 +2513,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -2016,7 +2521,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -2024,7 +2529,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -2032,7 +2537,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -2040,7 +2545,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -2048,7 +2553,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -2056,63 +2561,73 @@
         <v>254</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="20">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="3"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" ht="20">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="20">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" ht="20">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" ht="20">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="3"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" ht="20">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" ht="20">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="3"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -2120,31 +2635,36 @@
         <v>262</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="20">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="3"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" ht="20">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" ht="20">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="3"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -2152,7 +2672,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -2160,7 +2680,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -2168,15 +2688,17 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="20">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -2184,7 +2706,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -2192,7 +2714,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -2200,7 +2722,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -2208,7 +2730,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -2216,7 +2738,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -2224,7 +2746,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -2232,7 +2754,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -2240,7 +2762,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -2248,7 +2770,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -2256,7 +2778,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -2264,7 +2786,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -2272,7 +2794,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -2280,87 +2802,107 @@
         <v>276</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="20">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" s="3"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" ht="20">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95" s="3"/>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" ht="20">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" s="3"/>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" ht="20">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" s="3"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" ht="20">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" s="3"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" ht="20">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99" s="3"/>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" ht="20">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100" s="3"/>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" ht="20">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" s="3"/>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" ht="20">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102" s="3"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" ht="20">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" s="3"/>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -2368,7 +2910,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -2376,7 +2918,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -2384,7 +2926,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -2392,7 +2934,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -2400,7 +2942,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -2408,7 +2950,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -2416,7 +2958,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -2424,7 +2966,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -2432,7 +2974,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -2440,7 +2982,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -2448,7 +2990,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -2456,15 +2998,17 @@
         <v>302</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="20">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" s="3"/>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -2472,7 +3016,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -2480,7 +3024,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -2488,15 +3032,17 @@
         <v>306</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="20">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120" s="3"/>
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -2504,7 +3050,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -2512,7 +3058,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -2520,7 +3066,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -2528,7 +3074,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -2536,87 +3082,107 @@
         <v>312</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="20">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126" s="3"/>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" ht="20">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127" s="3"/>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" ht="20">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" s="3"/>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="1:4" ht="20">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" s="3"/>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4" ht="20">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" s="3"/>
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="1:4" ht="20">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131" s="3"/>
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="1:4" ht="20">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132" s="3"/>
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="1:4" ht="20">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133" s="3"/>
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134" spans="1:4" ht="20">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134" s="3"/>
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135" spans="1:4" ht="20">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135" s="3"/>
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -2624,7 +3190,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -2632,7 +3198,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -2640,7 +3206,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -2648,7 +3214,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -2656,7 +3222,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -2664,7 +3230,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -2672,7 +3238,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -2680,7 +3246,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -2688,7 +3254,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -2696,7 +3262,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -2704,7 +3270,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -2712,47 +3278,55 @@
         <v>334</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="20">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148" s="3"/>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:4" ht="20">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:4" ht="20">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150" s="3"/>
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="1:4" ht="20">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:4" ht="20">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152" s="3"/>
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -2760,7 +3334,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -2768,7 +3342,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -2776,7 +3350,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -2784,7 +3358,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -2792,7 +3366,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -2800,7 +3374,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -2808,7 +3382,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -2816,7 +3390,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -2824,7 +3398,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -2832,7 +3406,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -2840,7 +3414,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -2848,7 +3422,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -2856,7 +3430,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -2864,7 +3438,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -2872,7 +3446,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -2880,7 +3454,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -2888,135 +3462,167 @@
         <v>354</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="20">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170" s="3"/>
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171" spans="1:4" ht="20">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171" s="3"/>
+      <c r="D171" s="2"/>
+    </row>
+    <row r="172" spans="1:4" ht="20">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172" s="3"/>
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173" spans="1:4" ht="20">
       <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173" s="3"/>
+      <c r="D173" s="2"/>
+    </row>
+    <row r="174" spans="1:4" ht="20">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174" s="3"/>
+      <c r="D174" s="2"/>
+    </row>
+    <row r="175" spans="1:4" ht="20">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175" s="3"/>
+      <c r="D175" s="2"/>
+    </row>
+    <row r="176" spans="1:4" ht="20">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176" s="3"/>
+      <c r="D176" s="2"/>
+    </row>
+    <row r="177" spans="1:4" ht="20">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177" s="3"/>
+      <c r="D177" s="2"/>
+    </row>
+    <row r="178" spans="1:4" ht="20">
       <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178" s="3"/>
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179" spans="1:4" ht="20">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179" s="3"/>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="1:4" ht="20">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180" s="3"/>
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="1:4" ht="20">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181" s="3"/>
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="1:4" ht="20">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182" s="3"/>
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="1:4" ht="20">
       <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183" s="3"/>
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="1:4" ht="20">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184" s="3"/>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="1:4" ht="20">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185" s="3"/>
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -3024,7 +3630,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -3032,7 +3638,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -3040,7 +3646,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -3048,7 +3654,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -3056,12 +3662,850 @@
         <v>375</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>376</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="20">
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193" spans="3:3" ht="20">
+      <c r="C193" s="3"/>
+    </row>
+    <row r="194" spans="3:3" ht="20">
+      <c r="C194" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821A19C0-4F8C-8545-AB0F-03E6B9952E79}">
+  <dimension ref="A1:B78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
+  <cols>
+    <col min="1" max="1" width="29" style="12" customWidth="1"/>
+    <col min="2" max="2" width="65" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="34">
+      <c r="A40" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="34">
+      <c r="A50" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="34">
+      <c r="A51" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="34">
+      <c r="A55" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="34">
+      <c r="A56" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="9"/>
+      <c r="B74" s="7"/>
+    </row>
+    <row r="75" spans="1:2" ht="34">
+      <c r="A75" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="34">
+      <c r="A76" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="34">
+      <c r="A77" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="34">
+      <c r="A78" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42561DAC-25C1-EF43-9FFC-27DC3B436A8C}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="61.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="45.5" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28">
+      <c r="A1" s="15" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="43">
+      <c r="A2" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="21">
+      <c r="A3" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D3" s="20">
+        <v>44013</v>
+      </c>
+      <c r="E3" s="20">
+        <v>44926</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="21">
+      <c r="A4" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D4" s="20">
+        <v>44013</v>
+      </c>
+      <c r="E4" s="20">
+        <v>44926</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="21">
+      <c r="A5" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="20">
+        <v>44013</v>
+      </c>
+      <c r="E5" s="20">
+        <v>44926</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="21">
+      <c r="A6" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D6" s="20">
+        <v>44013</v>
+      </c>
+      <c r="E6" s="20">
+        <v>44926</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42">
+      <c r="A7" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="D7" s="20">
+        <v>43101</v>
+      </c>
+      <c r="E7" s="20">
+        <v>44012</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21">
+      <c r="A8" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D8" s="20">
+        <v>44013</v>
+      </c>
+      <c r="E8" s="20">
+        <v>44926</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21">
+      <c r="A9" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="20">
+        <v>43101</v>
+      </c>
+      <c r="E9" s="20">
+        <v>44012</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>